<commit_message>
New counterfactual and other changes
*effects by experience and counterfactual policy that eliminates experience restrictions
*fixed error in income formula
*new estimated parameters
</commit_message>
<xml_diff>
--- a/Outcomes.xlsx
+++ b/Outcomes.xlsx
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2.476491258370779</v>
+        <v>2.469545652167673</v>
       </c>
       <c r="E5" t="n">
         <v>2.473027724742889</v>
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.07297996026884278</v>
+        <v>0.0707115266285713</v>
       </c>
       <c r="E6" t="n">
         <v>0.07370234677940607</v>
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-0.3417941787759035</v>
+        <v>-0.3610816495766939</v>
       </c>
       <c r="E7" t="n">
         <v>-0.3557806353867054</v>
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.2262684439991096</v>
+        <v>0.2166748852961936</v>
       </c>
       <c r="E8" t="n">
         <v>0.2193343445211649</v>
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2.454719481739565</v>
+        <v>2.472840372559594</v>
       </c>
       <c r="E9" t="n">
         <v>2.589511615514755</v>
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.2835282793763605</v>
+        <v>0.2886132232229098</v>
       </c>
       <c r="E10" t="n">
         <v>0.3511904751360416</v>
@@ -649,7 +649,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2.445361585867946</v>
+        <v>2.433730285853511</v>
       </c>
       <c r="E11" t="n">
         <v>2.492676636982605</v>
@@ -678,7 +678,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.02204279370205894</v>
+        <v>0.01801372628179249</v>
       </c>
       <c r="E12" t="n">
         <v>0.03886315165764806</v>
@@ -707,7 +707,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.3709487283003633</v>
+        <v>0.3368671780379491</v>
       </c>
       <c r="E13" t="n">
         <v>0.282849339368839</v>
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.3613484053290271</v>
+        <v>0.3687202260799354</v>
       </c>
       <c r="E14" t="n">
         <v>0.5285899197979156</v>
@@ -765,7 +765,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.2256600726685506</v>
+        <v>0.256398869600323</v>
       </c>
       <c r="E15" t="n">
         <v>0.1486975891755972</v>
@@ -794,7 +794,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.2362069704323806</v>
+        <v>0.215621245755459</v>
       </c>
       <c r="E16" t="n">
         <v>0.2381999729142856</v>
@@ -823,7 +823,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.0580429263785073</v>
+        <v>0.1398250041155577</v>
       </c>
       <c r="E17" t="n">
         <v>0.2242346046674926</v>
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.01610557088551836</v>
+        <v>-0.01753936205462238</v>
       </c>
       <c r="E18" t="n">
         <v>-0.06573107417067822</v>
@@ -881,7 +881,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>-0.01576830739016967</v>
+        <v>0.003338890064221986</v>
       </c>
       <c r="E19" t="n">
         <v>-0.024197713692159</v>
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.4236162361623617</v>
+        <v>0.4428044280442804</v>
       </c>
       <c r="E20" t="n">
         <v>0.3770497444700439</v>
@@ -939,7 +939,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.0005606763686672347</v>
+        <v>0.0005665001879956587</v>
       </c>
       <c r="E21" t="n">
         <v>0.0007264937352508306</v>
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.4768307219455711</v>
+        <v>0.4818836742598442</v>
       </c>
       <c r="E22" t="n">
         <v>0.4184414642568783</v>
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.203601034335619</v>
+        <v>0.2404175451765602</v>
       </c>
       <c r="E23" t="n">
         <v>0.2074577010347085</v>

</xml_diff>

<commit_message>
New estimates and counterfactual
(i) New estimates that incorporates the modification of income.
(ii) Created new counterfactual experiment: lineal pay for performance, ATTs across baseline potential scores
</commit_message>
<xml_diff>
--- a/Outcomes.xlsx
+++ b/Outcomes.xlsx
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2.469545652167673</v>
+        <v>2.467451679673827</v>
       </c>
       <c r="E5" t="n">
         <v>2.473027724742889</v>
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.0707115266285713</v>
+        <v>0.0718444454608647</v>
       </c>
       <c r="E6" t="n">
         <v>0.07370234677940607</v>
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-0.3610816495766939</v>
+        <v>-0.364738004855809</v>
       </c>
       <c r="E7" t="n">
         <v>-0.3557806353867054</v>
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.2166748852961936</v>
+        <v>0.2165088495496961</v>
       </c>
       <c r="E8" t="n">
         <v>0.2193343445211649</v>
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2.472840372559594</v>
+        <v>2.471055733302607</v>
       </c>
       <c r="E9" t="n">
         <v>2.589511615514755</v>
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.2886132232229098</v>
+        <v>0.2870360540930463</v>
       </c>
       <c r="E10" t="n">
         <v>0.3511904751360416</v>
@@ -649,7 +649,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2.433730285853511</v>
+        <v>2.429455268249141</v>
       </c>
       <c r="E11" t="n">
         <v>2.492676636982605</v>
@@ -678,7 +678,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.01801372628179249</v>
+        <v>0.01868389180460234</v>
       </c>
       <c r="E12" t="n">
         <v>0.03886315165764806</v>
@@ -707,7 +707,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.3368671780379491</v>
+        <v>0.335123132821962</v>
       </c>
       <c r="E13" t="n">
         <v>0.282849339368839</v>
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.3687202260799354</v>
+        <v>0.3682034719418651</v>
       </c>
       <c r="E14" t="n">
         <v>0.5285899197979156</v>
@@ -765,7 +765,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.256398869600323</v>
+        <v>0.2579895034315705</v>
       </c>
       <c r="E15" t="n">
         <v>0.1486975891755972</v>
@@ -794,7 +794,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.215621245755459</v>
+        <v>0.2138775122646704</v>
       </c>
       <c r="E16" t="n">
         <v>0.2381999729142856</v>
@@ -823,7 +823,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.1398250041155577</v>
+        <v>0.1407421091689736</v>
       </c>
       <c r="E17" t="n">
         <v>0.2242346046674926</v>
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>-0.01753936205462238</v>
+        <v>-0.0190522757485441</v>
       </c>
       <c r="E18" t="n">
         <v>-0.06573107417067822</v>
@@ -881,7 +881,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.003338890064221986</v>
+        <v>0.003037414876917322</v>
       </c>
       <c r="E19" t="n">
         <v>-0.024197713692159</v>
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.4428044280442804</v>
+        <v>0.446931592392847</v>
       </c>
       <c r="E20" t="n">
         <v>0.3770497444700439</v>
@@ -939,7 +939,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.0005665001879956587</v>
+        <v>0.0005805021473523686</v>
       </c>
       <c r="E21" t="n">
         <v>0.0007264937352508306</v>
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.4818836742598442</v>
+        <v>0.4803335497809778</v>
       </c>
       <c r="E22" t="n">
         <v>0.4184414642568783</v>
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.2404175451765602</v>
+        <v>0.2416594240755823</v>
       </c>
       <c r="E23" t="n">
         <v>0.2074577010347085</v>

</xml_diff>

<commit_message>
fixed error in estimate
Fixed error in computation of a simulated moment
</commit_message>
<xml_diff>
--- a/Outcomes.xlsx
+++ b/Outcomes.xlsx
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2.467451679673827</v>
+        <v>2.485535850014337</v>
       </c>
       <c r="E5" t="n">
         <v>2.473027724742889</v>
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.0718444454608647</v>
+        <v>0.07175346706947595</v>
       </c>
       <c r="E6" t="n">
         <v>0.07370234677940607</v>
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-0.364738004855809</v>
+        <v>-0.2569518751681636</v>
       </c>
       <c r="E7" t="n">
         <v>-0.3557806353867054</v>
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.2165088495496961</v>
+        <v>0.2463665638042128</v>
       </c>
       <c r="E8" t="n">
         <v>0.2193343445211649</v>
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2.471055733302607</v>
+        <v>2.482289296325269</v>
       </c>
       <c r="E9" t="n">
         <v>2.589511615514755</v>
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.2870360540930463</v>
+        <v>0.2846642908342636</v>
       </c>
       <c r="E10" t="n">
         <v>0.3511904751360416</v>
@@ -649,7 +649,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2.429455268249141</v>
+        <v>2.454420695467284</v>
       </c>
       <c r="E11" t="n">
         <v>2.492676636982605</v>
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.446931592392847</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
         <v>0.3770497444700439</v>
@@ -939,7 +939,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.0005805021473523686</v>
+        <v>0.6261929753734357</v>
       </c>
       <c r="E21" t="n">
         <v>0.0007264937352508306</v>
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.4803335497809778</v>
+        <v>0.4671769704044489</v>
       </c>
       <c r="E22" t="n">
         <v>0.4184414642568783</v>
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.2416594240755823</v>
+        <v>0.1929157180451532</v>
       </c>
       <c r="E23" t="n">
         <v>0.2074577010347085</v>

</xml_diff>

<commit_message>
fixed errors in moments computation
</commit_message>
<xml_diff>
--- a/Outcomes.xlsx
+++ b/Outcomes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="data" sheetId="1" state="visible" r:id="rId1"/>
@@ -429,8 +429,8 @@
   </sheetPr>
   <dimension ref="C4:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J20" sqref="C20:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -475,13 +475,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2.485535850014337</v>
+        <v>2.486743561837384</v>
       </c>
       <c r="E5" t="n">
-        <v>2.473027724742889</v>
+        <v>2.473010797023773</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0783269219270539</v>
+        <v>0.07832692683838968</v>
       </c>
       <c r="G5" t="n">
         <v>0.5</v>
@@ -504,13 +504,13 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.07175346706947595</v>
+        <v>0.07191216137102167</v>
       </c>
       <c r="E6" t="n">
-        <v>0.07370234677940607</v>
+        <v>0.0737045496404171</v>
       </c>
       <c r="F6" t="n">
-        <v>0.002793042666449589</v>
+        <v>0.002791894768823342</v>
       </c>
       <c r="G6" t="n">
         <v>0.1</v>
@@ -533,13 +533,13 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-0.2569518751681636</v>
+        <v>-0.1763006811907082</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.3557806353867054</v>
+        <v>-0.3557592459619045</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01265455689849351</v>
+        <v>0.01269640106306268</v>
       </c>
       <c r="G7" t="n">
         <v>0.2</v>
@@ -562,13 +562,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.2463665638042128</v>
+        <v>0.3869429884421218</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2193343445211649</v>
+        <v>0.2193040450364351</v>
       </c>
       <c r="F8" t="n">
-        <v>0.008757212501268137</v>
+        <v>0.008640766787331089</v>
       </c>
       <c r="G8" t="n">
         <v>-0.01</v>
@@ -591,13 +591,13 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2.482289296325269</v>
+        <v>2.500736553924154</v>
       </c>
       <c r="E9" t="n">
-        <v>2.589511615514755</v>
+        <v>2.58952593588829</v>
       </c>
       <c r="F9" t="n">
-        <v>0.08229115197135939</v>
+        <v>0.08228883058330325</v>
       </c>
       <c r="G9" t="n">
         <v>0.1</v>
@@ -620,13 +620,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.2846642908342636</v>
+        <v>0.2858268679925717</v>
       </c>
       <c r="E10" t="n">
-        <v>0.3511904751360416</v>
+        <v>0.3511869743466377</v>
       </c>
       <c r="F10" t="n">
-        <v>0.01193093115858753</v>
+        <v>0.01197301821384926</v>
       </c>
       <c r="G10" t="n">
         <v>0.8</v>
@@ -649,13 +649,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2.454420695467284</v>
+        <v>2.464477557672385</v>
       </c>
       <c r="E11" t="n">
-        <v>2.492676636982605</v>
+        <v>2.492690888904214</v>
       </c>
       <c r="F11" t="n">
-        <v>0.07912521321515038</v>
+        <v>0.07911715410396938</v>
       </c>
       <c r="G11" t="n">
         <v>0.5</v>
@@ -678,13 +678,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.01868389180460234</v>
+        <v>0.01881308033911991</v>
       </c>
       <c r="E12" t="n">
-        <v>0.03886315165764806</v>
+        <v>0.0388672060009751</v>
       </c>
       <c r="F12" t="n">
-        <v>0.004045399688393174</v>
+        <v>0.004052441122115701</v>
       </c>
       <c r="G12" t="n">
         <v>0.1</v>
@@ -707,13 +707,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.335123132821962</v>
+        <v>0.3297214372224465</v>
       </c>
       <c r="E13" t="n">
-        <v>0.282849339368839</v>
+        <v>0.282855486013866</v>
       </c>
       <c r="F13" t="n">
-        <v>0.01310498917540976</v>
+        <v>0.01284582756155296</v>
       </c>
       <c r="G13" t="n">
         <v>0.2</v>
@@ -736,13 +736,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.3682034719418651</v>
+        <v>0.3625353249899071</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5285899197979156</v>
+        <v>0.5285845146094897</v>
       </c>
       <c r="F14" t="n">
-        <v>0.01962169850300514</v>
+        <v>0.01950110813856742</v>
       </c>
       <c r="G14" t="n">
         <v>-0.01</v>
@@ -765,13 +765,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.2579895034315705</v>
+        <v>0.2689301574485264</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1486975891755972</v>
+        <v>0.1486927933756691</v>
       </c>
       <c r="F15" t="n">
-        <v>0.008435343937196856</v>
+        <v>0.008571077048086666</v>
       </c>
       <c r="G15" t="n">
         <v>0.1</v>
@@ -794,13 +794,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.2138775122646704</v>
+        <v>0.2674542752462063</v>
       </c>
       <c r="E16" t="n">
-        <v>0.2381999729142856</v>
+        <v>0.2381824513994524</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0199206352053403</v>
+        <v>0.0193161450629829</v>
       </c>
       <c r="G16" t="n">
         <v>0.7</v>
@@ -823,13 +823,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.1407421091689736</v>
+        <v>0.1763744298772759</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2242346046674926</v>
+        <v>0.2242545439751264</v>
       </c>
       <c r="F17" t="n">
-        <v>0.02253028241901948</v>
+        <v>0.02157942660681845</v>
       </c>
       <c r="G17" t="n">
         <v>-0.4</v>
@@ -852,13 +852,13 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>-0.0190522757485441</v>
+        <v>-0.0125117225943009</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.06573107417067822</v>
+        <v>-0.06574915627640092</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0202643320763422</v>
+        <v>0.02065201320820884</v>
       </c>
       <c r="G18" t="n">
         <v>0.3</v>
@@ -881,13 +881,13 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.003037414876917322</v>
+        <v>-0.003802775894403772</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.024197713692159</v>
+        <v>-0.02422105296519655</v>
       </c>
       <c r="F19" t="n">
-        <v>0.02109193525631751</v>
+        <v>0.0203809442777414</v>
       </c>
       <c r="G19" t="n">
         <v>0.9</v>
@@ -913,10 +913,10 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.3770497444700439</v>
+        <v>0.3770313102118873</v>
       </c>
       <c r="F20" t="n">
-        <v>0.01446834731903008</v>
+        <v>0.01442944072430714</v>
       </c>
       <c r="G20" t="n">
         <v>1</v>
@@ -939,13 +939,13 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.6261929753734357</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0007264937352508306</v>
+        <v>0.585378801634811</v>
       </c>
       <c r="F21" t="n">
-        <v>4.265286409533425e-05</v>
+        <v>0.02020568064632542</v>
       </c>
       <c r="G21" t="n">
         <v>-0.1</v>
@@ -968,13 +968,13 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.4671769704044489</v>
+        <v>0.4657037156153698</v>
       </c>
       <c r="E22" t="n">
-        <v>0.4184414642568783</v>
+        <v>0.4184576788780685</v>
       </c>
       <c r="F22" t="n">
-        <v>0.01974929182721234</v>
+        <v>0.01973609522177048</v>
       </c>
       <c r="G22" t="n">
         <v>-0.2</v>
@@ -997,13 +997,13 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.1929157180451532</v>
+        <v>0.1967505437285323</v>
       </c>
       <c r="E23" t="n">
-        <v>0.2074577010347085</v>
+        <v>0.2073579741848141</v>
       </c>
       <c r="F23" t="n">
-        <v>0.01433207082703089</v>
+        <v>0.01427416787326762</v>
       </c>
       <c r="G23" t="n">
         <v>0.8</v>
@@ -1036,10 +1036,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:N22"/>
+  <dimension ref="B2:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:H22"/>
+    <sheetView zoomScale="144" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1231,7 +1231,7 @@
         <v/>
       </c>
       <c r="F11" s="12">
-        <f>data!E12*100</f>
+        <f>data!E12</f>
         <v/>
       </c>
       <c r="H11" s="14">
@@ -1250,7 +1250,7 @@
         <v/>
       </c>
       <c r="F12" s="12">
-        <f>data!E13*100</f>
+        <f>data!E13</f>
         <v/>
       </c>
       <c r="H12" s="14">
@@ -1269,7 +1269,7 @@
         <v/>
       </c>
       <c r="F13" s="12">
-        <f>data!E14*100</f>
+        <f>data!E14</f>
         <v/>
       </c>
       <c r="H13" s="14">
@@ -1289,7 +1289,7 @@
         <v/>
       </c>
       <c r="F14" s="12">
-        <f>data!E15*100</f>
+        <f>data!E15</f>
         <v/>
       </c>
       <c r="H14" s="14">
@@ -1384,7 +1384,7 @@
         <v/>
       </c>
       <c r="F19" s="12">
-        <f>data!E20*100</f>
+        <f>data!E20</f>
         <v/>
       </c>
       <c r="H19" s="14">
@@ -1404,7 +1404,7 @@
       </c>
       <c r="E20" s="15" t="n"/>
       <c r="F20" s="12">
-        <f>data!E21*100</f>
+        <f>data!E21</f>
         <v/>
       </c>
       <c r="G20" s="15" t="n"/>
@@ -1453,6 +1453,9 @@
         <f>data!F23</f>
         <v/>
       </c>
+    </row>
+    <row r="24">
+      <c r="F24" s="12" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes to utility and moments
*eliminate one moment
*change utility function
*added simce measure function
*fixed aep income
</commit_message>
<xml_diff>
--- a/Outcomes.xlsx
+++ b/Outcomes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="data" sheetId="1" state="visible" r:id="rId1"/>
@@ -427,10 +427,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C4:J24"/>
+  <dimension ref="C4:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J20" sqref="C20:J20"/>
+    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -475,13 +475,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2.486743561837384</v>
+        <v>2.439958992473283</v>
       </c>
       <c r="E5" t="n">
-        <v>2.473010797023773</v>
+        <v>2.473020242929459</v>
       </c>
       <c r="F5" t="n">
-        <v>0.07832692683838968</v>
+        <v>0.07832261502918832</v>
       </c>
       <c r="G5" t="n">
         <v>0.5</v>
@@ -504,13 +504,13 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.07191216137102167</v>
+        <v>0.06927355064914854</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0737045496404171</v>
+        <v>0.07376992758363485</v>
       </c>
       <c r="F6" t="n">
-        <v>0.002791894768823342</v>
+        <v>0.002756964555481807</v>
       </c>
       <c r="G6" t="n">
         <v>0.1</v>
@@ -533,13 +533,13 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-0.1763006811907082</v>
+        <v>-0.4475215708873302</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.3557592459619045</v>
+        <v>-0.3552965564727783</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01269640106306268</v>
+        <v>0.01283204546441114</v>
       </c>
       <c r="G7" t="n">
         <v>0.2</v>
@@ -562,13 +562,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.3869429884421218</v>
+        <v>0.1367171574465806</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2193040450364351</v>
+        <v>0.2189719285666943</v>
       </c>
       <c r="F8" t="n">
-        <v>0.008640766787331089</v>
+        <v>0.008714648232788468</v>
       </c>
       <c r="G8" t="n">
         <v>-0.01</v>
@@ -591,13 +591,13 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2.500736553924154</v>
+        <v>2.464592548098875</v>
       </c>
       <c r="E9" t="n">
-        <v>2.58952593588829</v>
+        <v>2.589592592477798</v>
       </c>
       <c r="F9" t="n">
-        <v>0.08228883058330325</v>
+        <v>0.08230323421738787</v>
       </c>
       <c r="G9" t="n">
         <v>0.1</v>
@@ -620,13 +620,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.2858268679925717</v>
+        <v>0.2942513028456653</v>
       </c>
       <c r="E10" t="n">
-        <v>0.3511869743466377</v>
+        <v>0.3511381005048752</v>
       </c>
       <c r="F10" t="n">
-        <v>0.01197301821384926</v>
+        <v>0.01203229253374716</v>
       </c>
       <c r="G10" t="n">
         <v>0.8</v>
@@ -649,13 +649,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2.464477557672385</v>
+        <v>2.418578590891703</v>
       </c>
       <c r="E11" t="n">
-        <v>2.492690888904214</v>
+        <v>2.492724134556088</v>
       </c>
       <c r="F11" t="n">
-        <v>0.07911715410396938</v>
+        <v>0.07914624579444615</v>
       </c>
       <c r="G11" t="n">
         <v>0.5</v>
@@ -678,13 +678,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.01881308033911991</v>
+        <v>0.02549858700040371</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0388672060009751</v>
+        <v>0.03895805112074458</v>
       </c>
       <c r="F12" t="n">
-        <v>0.004052441122115701</v>
+        <v>0.004028269770326015</v>
       </c>
       <c r="G12" t="n">
         <v>0.1</v>
@@ -707,13 +707,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.3297214372224465</v>
+        <v>0.3776907549454986</v>
       </c>
       <c r="E13" t="n">
-        <v>0.282855486013866</v>
+        <v>0.2825256499751223</v>
       </c>
       <c r="F13" t="n">
-        <v>0.01284582756155296</v>
+        <v>0.01278570880286808</v>
       </c>
       <c r="G13" t="n">
         <v>0.2</v>
@@ -736,13 +736,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.3625353249899071</v>
+        <v>0.3479127977392007</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5285845146094897</v>
+        <v>0.5282867442094009</v>
       </c>
       <c r="F14" t="n">
-        <v>0.01950110813856742</v>
+        <v>0.01946973085298174</v>
       </c>
       <c r="G14" t="n">
         <v>-0.01</v>
@@ -765,13 +765,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.2689301574485264</v>
+        <v>0.2288978603148971</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1486927933756691</v>
+        <v>0.1492295546947322</v>
       </c>
       <c r="F15" t="n">
-        <v>0.008571077048086666</v>
+        <v>0.008675134419246397</v>
       </c>
       <c r="G15" t="n">
         <v>0.1</v>
@@ -794,13 +794,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.2674542752462063</v>
+        <v>0.1569736613206976</v>
       </c>
       <c r="E16" t="n">
-        <v>0.2381824513994524</v>
+        <v>0.2381830824043836</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0193161450629829</v>
+        <v>0.01986858011483212</v>
       </c>
       <c r="G16" t="n">
         <v>0.7</v>
@@ -823,13 +823,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.1763744298772759</v>
+        <v>0.1666339721265211</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2242545439751264</v>
+        <v>0.2232180179692148</v>
       </c>
       <c r="F17" t="n">
-        <v>0.02157942660681845</v>
+        <v>0.02229085519208141</v>
       </c>
       <c r="G17" t="n">
         <v>-0.4</v>
@@ -852,13 +852,13 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>-0.0125117225943009</v>
+        <v>-0.0002070351378107086</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.06574915627640092</v>
+        <v>-0.06485860670546678</v>
       </c>
       <c r="F18" t="n">
-        <v>0.02065201320820884</v>
+        <v>0.01981038070346321</v>
       </c>
       <c r="G18" t="n">
         <v>0.3</v>
@@ -881,13 +881,13 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>-0.003802775894403772</v>
+        <v>-0.002116344328242216</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.02422105296519655</v>
+        <v>-0.02306611005363123</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0203809442777414</v>
+        <v>0.02042360966074426</v>
       </c>
       <c r="G19" t="n">
         <v>0.9</v>
@@ -909,27 +909,11 @@
           <t>\% Intermediate control</t>
         </is>
       </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.3770313102118873</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0.01442944072430714</v>
-      </c>
-      <c r="G20" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" t="n">
-        <v>15</v>
-      </c>
-      <c r="I20" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J20">
-        <f>(D20-E20)^2/F20^2</f>
-        <v/>
+      <c r="I20" s="3" t="n"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>ELIMINADO</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -939,13 +923,13 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>0.4730797615668464</v>
       </c>
       <c r="E21" t="n">
-        <v>0.585378801634811</v>
+        <v>0.5851949692469636</v>
       </c>
       <c r="F21" t="n">
-        <v>0.02020568064632542</v>
+        <v>0.02042369864481303</v>
       </c>
       <c r="G21" t="n">
         <v>-0.1</v>
@@ -968,13 +952,13 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.4657037156153698</v>
+        <v>0.4943662863465367</v>
       </c>
       <c r="E22" t="n">
-        <v>0.4184576788780685</v>
+        <v>0.4185176715820618</v>
       </c>
       <c r="F22" t="n">
-        <v>0.01973609522177048</v>
+        <v>0.01967542804872869</v>
       </c>
       <c r="G22" t="n">
         <v>-0.2</v>
@@ -997,13 +981,13 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.1967505437285323</v>
+        <v>0.247284977019973</v>
       </c>
       <c r="E23" t="n">
-        <v>0.2073579741848141</v>
+        <v>0.2080090161961711</v>
       </c>
       <c r="F23" t="n">
-        <v>0.01427416787326762</v>
+        <v>0.01423183394444534</v>
       </c>
       <c r="G23" t="n">
         <v>0.8</v>
@@ -1036,10 +1020,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:N24"/>
+  <dimension ref="B2:N23"/>
   <sheetViews>
-    <sheetView zoomScale="144" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1250,7 +1234,7 @@
         <v/>
       </c>
       <c r="F12" s="12">
-        <f>data!E13</f>
+        <f>data!E13*100</f>
         <v/>
       </c>
       <c r="H12" s="14">
@@ -1269,7 +1253,7 @@
         <v/>
       </c>
       <c r="F13" s="12">
-        <f>data!E14</f>
+        <f>data!E14*100</f>
         <v/>
       </c>
       <c r="H13" s="14">
@@ -1289,7 +1273,7 @@
         <v/>
       </c>
       <c r="F14" s="12">
-        <f>data!E15</f>
+        <f>data!E15*100</f>
         <v/>
       </c>
       <c r="H14" s="14">
@@ -1376,86 +1360,67 @@
     <row r="19">
       <c r="B19" t="inlineStr">
         <is>
-          <t>% intermediate (control group)</t>
+          <t>% advanced/expert (control group)</t>
         </is>
       </c>
       <c r="D19" s="12">
-        <f>data!D20*100</f>
-        <v/>
-      </c>
+        <f>data!D21*100</f>
+        <v/>
+      </c>
+      <c r="E19" s="15" t="n"/>
       <c r="F19" s="12">
-        <f>data!E20</f>
-        <v/>
-      </c>
+        <f>data!E21*100</f>
+        <v/>
+      </c>
+      <c r="G19" s="15" t="n"/>
       <c r="H19" s="14">
-        <f>data!F20*100</f>
+        <f>data!F21*100</f>
         <v/>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
-          <t>% advanced/expert (control group)</t>
+          <t>corr(STEI, past test scores)</t>
         </is>
       </c>
       <c r="D20" s="12">
-        <f>data!D21*100</f>
-        <v/>
-      </c>
-      <c r="E20" s="15" t="n"/>
+        <f>data!D22</f>
+        <v/>
+      </c>
       <c r="F20" s="12">
-        <f>data!E21</f>
-        <v/>
-      </c>
-      <c r="G20" s="15" t="n"/>
+        <f>data!E22</f>
+        <v/>
+      </c>
       <c r="H20" s="14">
-        <f>data!F21*100</f>
+        <f>data!F22</f>
         <v/>
       </c>
     </row>
     <row r="21">
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>corr(STEI, past test scores)</t>
-        </is>
-      </c>
-      <c r="D21" s="12">
-        <f>data!D22</f>
-        <v/>
-      </c>
-      <c r="F21" s="12">
-        <f>data!E22</f>
-        <v/>
-      </c>
-      <c r="H21" s="14">
-        <f>data!F22</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" s="4" t="inlineStr">
+      <c r="B21" s="4" t="inlineStr">
         <is>
           <t>corr(Portfolio,past test scores)</t>
         </is>
       </c>
-      <c r="C22" s="4" t="n"/>
-      <c r="D22" s="6">
+      <c r="C21" s="4" t="n"/>
+      <c r="D21" s="6">
         <f>data!D23</f>
         <v/>
       </c>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="6">
+      <c r="E21" s="5" t="n"/>
+      <c r="F21" s="6">
         <f>data!E23</f>
         <v/>
       </c>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="11">
+      <c r="G21" s="5" t="n"/>
+      <c r="H21" s="11">
         <f>data!F23</f>
         <v/>
       </c>
     </row>
-    <row r="24">
-      <c r="F24" s="12" t="n"/>
+    <row r="23">
+      <c r="F23" s="12" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes in utility 2
</commit_message>
<xml_diff>
--- a/Outcomes.xlsx
+++ b/Outcomes.xlsx
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2.439958992473283</v>
+        <v>2.496985546467907</v>
       </c>
       <c r="E5" t="n">
         <v>2.473020242929459</v>
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.06927355064914854</v>
+        <v>0.07635665951707242</v>
       </c>
       <c r="E6" t="n">
         <v>0.07376992758363485</v>
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-0.4475215708873302</v>
+        <v>-0.002535233822187239</v>
       </c>
       <c r="E7" t="n">
         <v>-0.3552965564727783</v>
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.1367171574465806</v>
+        <v>0.5400231511551582</v>
       </c>
       <c r="E8" t="n">
         <v>0.2189719285666943</v>
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2.464592548098875</v>
+        <v>2.533663549832727</v>
       </c>
       <c r="E9" t="n">
         <v>2.589592592477798</v>
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.2942513028456653</v>
+        <v>0.3030152403641788</v>
       </c>
       <c r="E10" t="n">
         <v>0.3511381005048752</v>
@@ -649,7 +649,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2.418578590891703</v>
+        <v>2.417443432035182</v>
       </c>
       <c r="E11" t="n">
         <v>2.492724134556088</v>
@@ -678,7 +678,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.02549858700040371</v>
+        <v>0.006475575292692774</v>
       </c>
       <c r="E12" t="n">
         <v>0.03895805112074458</v>
@@ -707,7 +707,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.3776907549454986</v>
+        <v>0.2025111021396851</v>
       </c>
       <c r="E13" t="n">
         <v>0.2825256499751223</v>
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.3479127977392007</v>
+        <v>0.3792894630601535</v>
       </c>
       <c r="E14" t="n">
         <v>0.5282867442094009</v>
@@ -765,7 +765,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.2288978603148971</v>
+        <v>0.3917238595074686</v>
       </c>
       <c r="E15" t="n">
         <v>0.1492295546947322</v>
@@ -794,7 +794,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.1569736613206976</v>
+        <v>0.03537009864606364</v>
       </c>
       <c r="E16" t="n">
         <v>0.2381830824043836</v>
@@ -823,7 +823,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.1666339721265211</v>
+        <v>0.01064639444370955</v>
       </c>
       <c r="E17" t="n">
         <v>0.2232180179692148</v>
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>-0.0002070351378107086</v>
+        <v>-0.06424314580939124</v>
       </c>
       <c r="E18" t="n">
         <v>-0.06485860670546678</v>
@@ -881,7 +881,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>-0.002116344328242216</v>
+        <v>-0.02792184497684371</v>
       </c>
       <c r="E19" t="n">
         <v>-0.02306611005363123</v>
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.4730797615668464</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
         <v>0.5851949692469636</v>
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.4943662863465367</v>
+        <v>0.5067639732573387</v>
       </c>
       <c r="E22" t="n">
         <v>0.4185176715820618</v>
@@ -981,7 +981,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.247284977019973</v>
+        <v>0.2651495670929225</v>
       </c>
       <c r="E23" t="n">
         <v>0.2080090161961711</v>

</xml_diff>

<commit_message>
Moment for treatment group
Correlation of past test scores with current portfolio and examen measures only for treatment group
</commit_message>
<xml_diff>
--- a/Outcomes.xlsx
+++ b/Outcomes.xlsx
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2.473080877566929</v>
+        <v>2.490706599329265</v>
       </c>
       <c r="E5" t="n">
         <v>2.473205427646637</v>
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.07089260008814578</v>
+        <v>0.06892690360037453</v>
       </c>
       <c r="E6" t="n">
         <v>0.0736510165631771</v>
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-0.4303515706337896</v>
+        <v>-0.3633355102425982</v>
       </c>
       <c r="E7" t="n">
         <v>-0.3556503586471081</v>
@@ -564,7 +564,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.2531835998636042</v>
+        <v>0.2290779302062357</v>
       </c>
       <c r="E8" t="n">
         <v>0.2194834295511246</v>
@@ -593,7 +593,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2.584361381911414</v>
+        <v>2.513774459734022</v>
       </c>
       <c r="E9" t="n">
         <v>2.589686144113541</v>
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.2897028536153853</v>
+        <v>0.295579317546473</v>
       </c>
       <c r="E10" t="n">
         <v>0.3512575879693031</v>
@@ -651,7 +651,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2.549817094759991</v>
+        <v>2.515486904511018</v>
       </c>
       <c r="E11" t="n">
         <v>2.492827641489762</v>
@@ -680,7 +680,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.3488171174808235</v>
+        <v>0.3455551069842551</v>
       </c>
       <c r="E12" t="n">
         <v>0.2823352706700801</v>
@@ -709,7 +709,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.3750827614049252</v>
+        <v>0.3855308841340331</v>
       </c>
       <c r="E13" t="n">
         <v>0.5282260225785356</v>
@@ -738,7 +738,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.2160113039967703</v>
+        <v>0.2158901897456601</v>
       </c>
       <c r="E14" t="n">
         <v>0.149058450399161</v>
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.08046532556029756</v>
+        <v>0.2375479266643894</v>
       </c>
       <c r="E15" t="n">
         <v>0.2388526880499385</v>
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.03514255336468614</v>
+        <v>0.1209527201462497</v>
       </c>
       <c r="E16" t="n">
         <v>0.22419319888022</v>
@@ -825,7 +825,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>-0.12658406026969</v>
+        <v>-0.08396974945207074</v>
       </c>
       <c r="E17" t="n">
         <v>-0.06540378725536067</v>
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>-0.02043483727125512</v>
+        <v>-0.01276729934991094</v>
       </c>
       <c r="E18" t="n">
         <v>-0.02392661882078389</v>
@@ -883,7 +883,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.6445699687766109</v>
+        <v>0.6212943514050525</v>
       </c>
       <c r="E19" t="n">
         <v>0.585264909228308</v>
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.4129786342362503</v>
+        <v>0.3830234347913151</v>
       </c>
       <c r="E20" t="n">
         <v>0.4185593185121093</v>
@@ -941,7 +941,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.2116097385582484</v>
+        <v>0.1789474868051397</v>
       </c>
       <c r="E21" t="n">
         <v>0.208091256202629</v>
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>-0.0764580810336728</v>
+        <v>0.02360350061983014</v>
       </c>
       <c r="E22" t="n">
         <v>0.006995364946533139</v>

</xml_diff>

<commit_message>
Moment for control group
Fixed moment construction for control group. It was using treatment-group placement instead of AEP.
</commit_message>
<xml_diff>
--- a/Outcomes.xlsx
+++ b/Outcomes.xlsx
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2.490706599329265</v>
+        <v>2.471205793740484</v>
       </c>
       <c r="E5" t="n">
         <v>2.473205427646637</v>
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.06892690360037453</v>
+        <v>0.06871335925147376</v>
       </c>
       <c r="E6" t="n">
         <v>0.0736510165631771</v>
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-0.3633355102425982</v>
+        <v>-0.4023230641462986</v>
       </c>
       <c r="E7" t="n">
         <v>-0.3556503586471081</v>
@@ -564,7 +564,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.2290779302062357</v>
+        <v>0.09566701766772445</v>
       </c>
       <c r="E8" t="n">
         <v>0.2194834295511246</v>
@@ -593,7 +593,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2.513774459734022</v>
+        <v>2.45035931757805</v>
       </c>
       <c r="E9" t="n">
         <v>2.589686144113541</v>
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.295579317546473</v>
+        <v>0.2911811583879726</v>
       </c>
       <c r="E10" t="n">
         <v>0.3512575879693031</v>
@@ -651,7 +651,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2.515486904511018</v>
+        <v>2.475610245698677</v>
       </c>
       <c r="E11" t="n">
         <v>2.492827641489762</v>
@@ -680,7 +680,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.3455551069842551</v>
+        <v>0.389430763019782</v>
       </c>
       <c r="E12" t="n">
         <v>0.2823352706700801</v>
@@ -709,7 +709,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.3855308841340331</v>
+        <v>0.3735002018570852</v>
       </c>
       <c r="E13" t="n">
         <v>0.5282260225785356</v>
@@ -738,7 +738,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.2158901897456601</v>
+        <v>0.178700040371417</v>
       </c>
       <c r="E14" t="n">
         <v>0.149058450399161</v>
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.2375479266643894</v>
+        <v>0.3641247559069888</v>
       </c>
       <c r="E15" t="n">
         <v>0.2388526880499385</v>
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.1209527201462497</v>
+        <v>0.06189974787140653</v>
       </c>
       <c r="E16" t="n">
         <v>0.22419319888022</v>
@@ -825,7 +825,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>-0.08396974945207074</v>
+        <v>-0.1046421997387022</v>
       </c>
       <c r="E17" t="n">
         <v>-0.06540378725536067</v>
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>-0.01276729934991094</v>
+        <v>-0.01432397469862057</v>
       </c>
       <c r="E18" t="n">
         <v>-0.02392661882078389</v>
@@ -883,7 +883,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.6212943514050525</v>
+        <v>0.6225887028101049</v>
       </c>
       <c r="E19" t="n">
         <v>0.585264909228308</v>
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.3830234347913151</v>
+        <v>0.3868634900551436</v>
       </c>
       <c r="E20" t="n">
         <v>0.4185593185121093</v>
@@ -941,7 +941,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.1789474868051397</v>
+        <v>0.2096526231084588</v>
       </c>
       <c r="E21" t="n">
         <v>0.208091256202629</v>
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.02360350061983014</v>
+        <v>-0.02340715085628979</v>
       </c>
       <c r="E22" t="n">
         <v>0.006995364946533139</v>

</xml_diff>

<commit_message>
Included two new moments
Included two new moments: regression of probability of expert on past test score (either portfolio or test)
</commit_message>
<xml_diff>
--- a/Outcomes.xlsx
+++ b/Outcomes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4780" yWindow="500" windowWidth="28800" windowHeight="16300" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="data" sheetId="1" state="visible" r:id="rId1"/>
@@ -437,10 +437,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C4:J23"/>
+  <dimension ref="C4:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -485,13 +485,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2.356137804814221</v>
+        <v>2.464088200842154</v>
       </c>
       <c r="E5" t="n">
-        <v>2.581629552841187</v>
+        <v>2.581198556184769</v>
       </c>
       <c r="F5" t="n">
-        <v>0.08183032940787834</v>
+        <v>0.08182810964922846</v>
       </c>
       <c r="G5" t="n">
         <v>0.5</v>
@@ -514,13 +514,13 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.06525573625019801</v>
+        <v>0.06927044459805856</v>
       </c>
       <c r="E6" t="n">
-        <v>0.06258531584590674</v>
+        <v>0.06250998651981354</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00281639474968377</v>
+        <v>0.002812108107274512</v>
       </c>
       <c r="G6" t="n">
         <v>0.1</v>
@@ -543,13 +543,13 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-0.3439002818042596</v>
+        <v>-0.3994801237015926</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.3443836978673935</v>
+        <v>-0.3443212494254112</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01143701077400334</v>
+        <v>0.01137968585875859</v>
       </c>
       <c r="G7" t="n">
         <v>0.2</v>
@@ -572,13 +572,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.2311914922271492</v>
+        <v>0.2199161972911622</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2285009965449572</v>
+        <v>0.2285554205775261</v>
       </c>
       <c r="F8" t="n">
-        <v>0.007784128407898858</v>
+        <v>0.007737233353145483</v>
       </c>
       <c r="G8" t="n">
         <v>-0.01</v>
@@ -601,13 +601,13 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2.515728496350382</v>
+        <v>2.509349917307424</v>
       </c>
       <c r="E9" t="n">
-        <v>2.592340103149414</v>
+        <v>2.592065150976181</v>
       </c>
       <c r="F9" t="n">
-        <v>0.08270686259312163</v>
+        <v>0.08266076218085858</v>
       </c>
       <c r="G9" t="n">
         <v>0.1</v>
@@ -630,13 +630,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.273670527879375</v>
+        <v>0.2905799883187443</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2634404433369636</v>
+        <v>0.2635648551732302</v>
       </c>
       <c r="F10" t="n">
-        <v>0.01059491003840474</v>
+        <v>0.01053098017579399</v>
       </c>
       <c r="G10" t="n">
         <v>0.8</v>
@@ -659,13 +659,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2.432198079641796</v>
+        <v>2.490999063512804</v>
       </c>
       <c r="E11" t="n">
-        <v>2.410675540180921</v>
+        <v>2.410592958283658</v>
       </c>
       <c r="F11" t="n">
-        <v>0.07630885580160061</v>
+        <v>0.07631052784374842</v>
       </c>
       <c r="G11" t="n">
         <v>0.5</v>
@@ -688,13 +688,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.3120016174686616</v>
+        <v>0.3616012939749292</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2817199851640899</v>
+        <v>0.2821355535332045</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01270233237277591</v>
+        <v>0.01259466476202391</v>
       </c>
       <c r="G12" t="n">
         <v>0.2</v>
@@ -717,13 +717,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.4421431459765467</v>
+        <v>0.3817226041245452</v>
       </c>
       <c r="E13" t="n">
-        <v>0.5291691092703767</v>
+        <v>0.529291248397036</v>
       </c>
       <c r="F13" t="n">
-        <v>0.01963339001921008</v>
+        <v>0.01947491925114392</v>
       </c>
       <c r="G13" t="n">
         <v>-0.01</v>
@@ -746,13 +746,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.1833885968459361</v>
+        <v>0.1826202992317024</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1491808168279789</v>
+        <v>0.1488150260894422</v>
       </c>
       <c r="F14" t="n">
-        <v>0.008747560962337361</v>
+        <v>0.008497317180154439</v>
       </c>
       <c r="G14" t="n">
         <v>0.1</v>
@@ -775,13 +775,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.2421704917092923</v>
+        <v>0.2224529920915002</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2400210314531001</v>
+        <v>0.2389975308689028</v>
       </c>
       <c r="F15" t="n">
-        <v>0.02046209715376685</v>
+        <v>0.01970719446538374</v>
       </c>
       <c r="G15" t="n">
         <v>0.7</v>
@@ -804,13 +804,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.171222256034539</v>
+        <v>0.1164375179339663</v>
       </c>
       <c r="E16" t="n">
-        <v>0.2268727637985438</v>
+        <v>0.226189139557443</v>
       </c>
       <c r="F16" t="n">
-        <v>0.02170374319004783</v>
+        <v>0.02150634078225261</v>
       </c>
       <c r="G16" t="n">
         <v>-0.4</v>
@@ -833,13 +833,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>-0.2233103409440996</v>
+        <v>-0.07164023951563281</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.0661008244831439</v>
+        <v>-0.06684177619523311</v>
       </c>
       <c r="F17" t="n">
-        <v>0.02014208879289298</v>
+        <v>0.02030145292122476</v>
       </c>
       <c r="G17" t="n">
         <v>0.3</v>
@@ -862,13 +862,13 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>-0.03217970150651106</v>
+        <v>-0.01872787656146262</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.02651057771846508</v>
+        <v>-0.02534243929760681</v>
       </c>
       <c r="F18" t="n">
-        <v>0.01991254957604298</v>
+        <v>0.02070464178194394</v>
       </c>
       <c r="G18" t="n">
         <v>0.9</v>
@@ -891,13 +891,13 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.4468211274875265</v>
+        <v>0.5639777484659059</v>
       </c>
       <c r="E19" t="n">
-        <v>0.3160884780617422</v>
+        <v>0.3161279605158629</v>
       </c>
       <c r="F19" t="n">
-        <v>0.01057443201292244</v>
+        <v>0.01064494658365078</v>
       </c>
       <c r="G19" t="n">
         <v>-0.1</v>
@@ -920,13 +920,13 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.6215673390842769</v>
+        <v>0.4813890666782157</v>
       </c>
       <c r="E20" t="n">
-        <v>0.5886643553724413</v>
+        <v>0.588282594848905</v>
       </c>
       <c r="F20" t="n">
-        <v>0.02423126045368539</v>
+        <v>0.02417879833631291</v>
       </c>
       <c r="G20" t="n">
         <v>-0.2</v>
@@ -949,13 +949,13 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.2775019744116156</v>
+        <v>0.2215609137065696</v>
       </c>
       <c r="E21" t="n">
-        <v>0.3238487507075737</v>
+        <v>0.3246538201806384</v>
       </c>
       <c r="F21" t="n">
-        <v>0.02046718181772308</v>
+        <v>0.02109262303944222</v>
       </c>
       <c r="G21" t="n">
         <v>0.8</v>
@@ -978,13 +978,13 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.0477047466939745</v>
+        <v>-0.05634598840963018</v>
       </c>
       <c r="E22" t="n">
-        <v>0.04068252310754032</v>
+        <v>0.04015706062279335</v>
       </c>
       <c r="F22" t="n">
-        <v>0.007304322614855204</v>
+        <v>0.007065554505528104</v>
       </c>
       <c r="J22">
         <f>(D22-E22)^2/F22^2</f>
@@ -992,8 +992,32 @@
       </c>
     </row>
     <row r="23">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Past portfolio and % expert</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v/>
+      </c>
+      <c r="F23" t="n">
+        <v/>
+      </c>
       <c r="J23">
         <f>SUM(J5:J22)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Past test and % expert</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v/>
+      </c>
+      <c r="F24" t="n">
         <v/>
       </c>
     </row>
@@ -1526,8 +1550,8 @@
   </sheetPr>
   <dimension ref="B2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1868,7 +1892,7 @@
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
-          <t>Mean Portfolio-Test (control)</t>
+          <t>Average of past portfolio-test (control)</t>
         </is>
       </c>
       <c r="D20" s="14">

</xml_diff>

<commit_message>
Estimation of model with new salary components
</commit_message>
<xml_diff>
--- a/Outcomes.xlsx
+++ b/Outcomes.xlsx
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2.393049952958328</v>
+        <v>2.363070468628005</v>
       </c>
       <c r="E5" t="n">
         <v>2.581565579414367</v>
@@ -514,7 +514,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.06728785659685134</v>
+        <v>0.07188899101417243</v>
       </c>
       <c r="E6" t="n">
         <v>0.06257367359101772</v>
@@ -543,7 +543,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-0.2642008424161997</v>
+        <v>-0.3481388986083073</v>
       </c>
       <c r="E7" t="n">
         <v>-0.3444480294585228</v>
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.24336377555324</v>
+        <v>0.2262012405916103</v>
       </c>
       <c r="E8" t="n">
         <v>0.2285021986961365</v>
@@ -601,7 +601,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2.507219055660872</v>
+        <v>2.492867487854896</v>
       </c>
       <c r="E9" t="n">
         <v>2.592231221914291</v>
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.2630387394224682</v>
+        <v>0.2671958650971716</v>
       </c>
       <c r="E10" t="n">
         <v>0.263034506380558</v>
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2.442980255682476</v>
+        <v>2.418529064907384</v>
       </c>
       <c r="E11" t="n">
         <v>2.410472437144871</v>
@@ -688,7 +688,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.3046097856854023</v>
+        <v>0.3311118621155796</v>
       </c>
       <c r="E12" t="n">
         <v>0.2818777895815746</v>
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.4334977759805904</v>
+        <v>0.4266508955728286</v>
       </c>
       <c r="E13" t="n">
         <v>0.5296577431267996</v>
@@ -746,7 +746,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.2133117670845127</v>
+        <v>0.2009665427509293</v>
       </c>
       <c r="E14" t="n">
         <v>0.1488104173512825</v>
@@ -775,7 +775,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.1812050472975702</v>
+        <v>0.2336306198937148</v>
       </c>
       <c r="E15" t="n">
         <v>0.2386545155406662</v>
@@ -804,7 +804,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.3620695402176274</v>
+        <v>0.2780790558736198</v>
       </c>
       <c r="E16" t="n">
         <v>0.2260111108603461</v>
@@ -833,7 +833,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>-0.09692319278094491</v>
+        <v>-0.1564787544150041</v>
       </c>
       <c r="E17" t="n">
         <v>-0.06602769124240029</v>
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.01539010981703655</v>
+        <v>0.005974167488294789</v>
       </c>
       <c r="E18" t="n">
         <v>-0.02509134328193019</v>
@@ -891,7 +891,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.4720880885473419</v>
+        <v>0.4117376532571767</v>
       </c>
       <c r="E19" t="n">
         <v>0.3160005902945181</v>
@@ -920,7 +920,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.6554887257281814</v>
+        <v>0.6240486996118719</v>
       </c>
       <c r="E20" t="n">
         <v>0.5879475685821897</v>
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.1353599220474271</v>
+        <v>0.2237575135350566</v>
       </c>
       <c r="E21" t="n">
         <v>0.3237328135489578</v>
@@ -978,7 +978,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.1208231616059848</v>
+        <v>0.03675178589910508</v>
       </c>
       <c r="E22" t="n">
         <v>0.04067292148046374</v>
@@ -998,7 +998,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.2355367723246737</v>
+        <v>0.2366326647980964</v>
       </c>
       <c r="E23" t="n">
         <v>0.3823872146348747</v>
@@ -1018,7 +1018,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.3251983326596373</v>
+        <v>0.3266854758224005</v>
       </c>
       <c r="E24" t="n">
         <v>0.4946261909055633</v>

</xml_diff>

<commit_message>
Back to simpler utility function
Utility function with no interactions
</commit_message>
<xml_diff>
--- a/Outcomes.xlsx
+++ b/Outcomes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="data" sheetId="1" state="visible" r:id="rId1"/>
@@ -437,10 +437,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C4:J25"/>
+  <dimension ref="C4:J23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -485,13 +485,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2.363070468628005</v>
+        <v>2.373420435428225</v>
       </c>
       <c r="E5" t="n">
-        <v>2.581565579414367</v>
+        <v>2.576630519628525</v>
       </c>
       <c r="F5" t="n">
-        <v>0.08182874260292955</v>
+        <v>0.08164715903196171</v>
       </c>
       <c r="G5" t="n">
         <v>0.5</v>
@@ -514,13 +514,13 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.07188899101417243</v>
+        <v>0.07138971453727255</v>
       </c>
       <c r="E6" t="n">
-        <v>0.06257367359101772</v>
+        <v>0.06133794514834881</v>
       </c>
       <c r="F6" t="n">
-        <v>0.002818761422043914</v>
+        <v>0.002622678095011646</v>
       </c>
       <c r="G6" t="n">
         <v>0.1</v>
@@ -543,13 +543,13 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-0.3481388986083073</v>
+        <v>-0.3388462548494522</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.3444480294585228</v>
+        <v>-0.3525642129778862</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01140426822338832</v>
+        <v>0.01161199713255933</v>
       </c>
       <c r="G7" t="n">
         <v>0.2</v>
@@ -572,13 +572,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.2262012405916103</v>
+        <v>0.2288157473547942</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2285021986961365</v>
+        <v>0.2638800442814827</v>
       </c>
       <c r="F8" t="n">
-        <v>0.007768222776008471</v>
+        <v>0.008885795218818177</v>
       </c>
       <c r="G8" t="n">
         <v>-0.01</v>
@@ -601,13 +601,13 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2.492867487854896</v>
+        <v>2.493656150024008</v>
       </c>
       <c r="E9" t="n">
-        <v>2.592231221914291</v>
+        <v>2.585287255048752</v>
       </c>
       <c r="F9" t="n">
-        <v>0.08266344020207321</v>
+        <v>0.08235110389677236</v>
       </c>
       <c r="G9" t="n">
         <v>0.1</v>
@@ -630,13 +630,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.2671958650971716</v>
+        <v>0.2646393723224644</v>
       </c>
       <c r="E10" t="n">
-        <v>0.263034506380558</v>
+        <v>0.2584711409658194</v>
       </c>
       <c r="F10" t="n">
-        <v>0.01048503481222027</v>
+        <v>0.01004802869067144</v>
       </c>
       <c r="G10" t="n">
         <v>0.8</v>
@@ -659,13 +659,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2.418529064907384</v>
+        <v>2.423554827489142</v>
       </c>
       <c r="E11" t="n">
-        <v>2.410472437144871</v>
+        <v>2.4094847646897</v>
       </c>
       <c r="F11" t="n">
-        <v>0.07630338103185176</v>
+        <v>0.07626731252655336</v>
       </c>
       <c r="G11" t="n">
         <v>0.5</v>
@@ -688,13 +688,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.3311118621155796</v>
+        <v>0.309205812774586</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2818777895815746</v>
+        <v>0.2851554799245871</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01260738185948163</v>
+        <v>0.0121985665418822</v>
       </c>
       <c r="G12" t="n">
         <v>0.2</v>
@@ -717,13 +717,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.4266508955728286</v>
+        <v>0.4515444406894221</v>
       </c>
       <c r="E13" t="n">
-        <v>0.5296577431267996</v>
+        <v>0.5315983342694378</v>
       </c>
       <c r="F13" t="n">
-        <v>0.01947581392868195</v>
+        <v>0.01916980495591796</v>
       </c>
       <c r="G13" t="n">
         <v>-0.01</v>
@@ -746,13 +746,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.2009665427509293</v>
+        <v>0.199905373436972</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1488104173512825</v>
+        <v>0.1418508460156945</v>
       </c>
       <c r="F14" t="n">
-        <v>0.008389467782156297</v>
+        <v>0.007941641941221683</v>
       </c>
       <c r="G14" t="n">
         <v>0.1</v>
@@ -775,13 +775,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.2336306198937148</v>
+        <v>0.1888404246655233</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2386545155406662</v>
+        <v>0.2068904141768755</v>
       </c>
       <c r="F15" t="n">
-        <v>0.02023419711379746</v>
+        <v>0.01885783011450599</v>
       </c>
       <c r="G15" t="n">
         <v>0.7</v>
@@ -804,13 +804,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.2780790558736198</v>
+        <v>0.2378275213560124</v>
       </c>
       <c r="E16" t="n">
-        <v>0.2260111108603461</v>
+        <v>0.2015302385505502</v>
       </c>
       <c r="F16" t="n">
-        <v>0.02186858751736081</v>
+        <v>0.01968563812959444</v>
       </c>
       <c r="G16" t="n">
         <v>-0.4</v>
@@ -833,13 +833,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>-0.1564787544150041</v>
+        <v>-0.1448787886555005</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.06602769124240029</v>
+        <v>-0.05900479096240778</v>
       </c>
       <c r="F17" t="n">
-        <v>0.02050401360225442</v>
+        <v>0.01803628546388143</v>
       </c>
       <c r="G17" t="n">
         <v>0.3</v>
@@ -862,13 +862,13 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.005974167488294789</v>
+        <v>0.00759650508292628</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.02509134328193019</v>
+        <v>-0.02479339063389524</v>
       </c>
       <c r="F18" t="n">
-        <v>0.02006525571072114</v>
+        <v>0.01834683408094412</v>
       </c>
       <c r="G18" t="n">
         <v>0.9</v>
@@ -891,13 +891,13 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.4117376532571767</v>
+        <v>0.4211344724013983</v>
       </c>
       <c r="E19" t="n">
-        <v>0.3160005902945181</v>
+        <v>0.3169023398360751</v>
       </c>
       <c r="F19" t="n">
-        <v>0.01058874699875399</v>
+        <v>0.01053797245042425</v>
       </c>
       <c r="G19" t="n">
         <v>-0.1</v>
@@ -920,13 +920,13 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.6240486996118719</v>
+        <v>0.6191579988240159</v>
       </c>
       <c r="E20" t="n">
-        <v>0.5879475685821897</v>
+        <v>0.5795648185578327</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0240041724868178</v>
+        <v>0.02327032290503902</v>
       </c>
       <c r="G20" t="n">
         <v>-0.2</v>
@@ -949,13 +949,13 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.2237575135350566</v>
+        <v>0.1102882946930028</v>
       </c>
       <c r="E21" t="n">
-        <v>0.3237328135489578</v>
+        <v>0.3111629186435975</v>
       </c>
       <c r="F21" t="n">
-        <v>0.02075877695300378</v>
+        <v>0.01953587741858369</v>
       </c>
       <c r="G21" t="n">
         <v>0.8</v>
@@ -978,13 +978,13 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.03675178589910508</v>
+        <v>0.02474953602968901</v>
       </c>
       <c r="E22" t="n">
-        <v>0.04067292148046374</v>
+        <v>0.03398225929140364</v>
       </c>
       <c r="F22" t="n">
-        <v>0.007255925061936016</v>
+        <v>0.006352793746508848</v>
       </c>
       <c r="J22">
         <f>(D22-E22)^2/F22^2</f>
@@ -992,48 +992,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Past portfolio and % expert</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>0.2366326647980964</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.3823872146348747</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.02030854832062191</v>
-      </c>
       <c r="J23">
-        <f>(D23-E23)^2/F23^2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24">
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Past test and % expert</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>0.3266854758224005</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.4946261909055633</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0.02262665737790864</v>
-      </c>
-      <c r="J24">
-        <f>(D24-E24)^2/F24^2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25">
-      <c r="J25">
-        <f>SUM(J5:J24)</f>
+        <f>SUM(J5:J22)</f>
         <v/>
       </c>
     </row>
@@ -1566,8 +1526,8 @@
   </sheetPr>
   <dimension ref="B2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Updated fit and counterfactual
Updated fit and counterfactual experiments to the new model and estimates
</commit_message>
<xml_diff>
--- a/Outcomes.xlsx
+++ b/Outcomes.xlsx
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2.373420435428225</v>
+        <v>2.367899673874997</v>
       </c>
       <c r="E5" t="n">
         <v>2.576630519628525</v>
@@ -514,7 +514,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.07138971453727255</v>
+        <v>0.07002404621610055</v>
       </c>
       <c r="E6" t="n">
         <v>0.06133794514834881</v>
@@ -543,7 +543,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-0.3388462548494522</v>
+        <v>-0.3559151560458474</v>
       </c>
       <c r="E7" t="n">
         <v>-0.3525642129778862</v>
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.2288157473547942</v>
+        <v>0.2619431526596601</v>
       </c>
       <c r="E8" t="n">
         <v>0.2638800442814827</v>
@@ -601,7 +601,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2.493656150024008</v>
+        <v>2.498394558263731</v>
       </c>
       <c r="E9" t="n">
         <v>2.585287255048752</v>
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.2646393723224644</v>
+        <v>0.2530015216472968</v>
       </c>
       <c r="E10" t="n">
         <v>0.2584711409658194</v>
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2.423554827489142</v>
+        <v>2.42295084177452</v>
       </c>
       <c r="E11" t="n">
         <v>2.4094847646897</v>
@@ -688,7 +688,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.309205812774586</v>
+        <v>0.3224670496789456</v>
       </c>
       <c r="E12" t="n">
         <v>0.2851554799245871</v>
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.4515444406894221</v>
+        <v>0.4435958093950659</v>
       </c>
       <c r="E13" t="n">
         <v>0.5315983342694378</v>
@@ -746,7 +746,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.199905373436972</v>
+        <v>0.1936870564379858</v>
       </c>
       <c r="E14" t="n">
         <v>0.1418508460156945</v>
@@ -775,7 +775,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.1888404246655233</v>
+        <v>0.193282093897509</v>
       </c>
       <c r="E15" t="n">
         <v>0.2068904141768755</v>
@@ -804,7 +804,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.2378275213560124</v>
+        <v>0.219220690029325</v>
       </c>
       <c r="E16" t="n">
         <v>0.2015302385505502</v>
@@ -833,7 +833,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>-0.1448787886555005</v>
+        <v>-0.1105923956464526</v>
       </c>
       <c r="E17" t="n">
         <v>-0.05900479096240778</v>
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.00759650508292628</v>
+        <v>0.005863903358051403</v>
       </c>
       <c r="E18" t="n">
         <v>-0.02479339063389524</v>
@@ -891,7 +891,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.4211344724013983</v>
+        <v>0.4143630902555517</v>
       </c>
       <c r="E19" t="n">
         <v>0.3169023398360751</v>
@@ -920,7 +920,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.6191579988240159</v>
+        <v>0.5139108704465918</v>
       </c>
       <c r="E20" t="n">
         <v>0.5795648185578327</v>
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.1102882946930028</v>
+        <v>0.1719286908784542</v>
       </c>
       <c r="E21" t="n">
         <v>0.3111629186435975</v>
@@ -978,7 +978,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.02474953602968901</v>
+        <v>0.03066205678034255</v>
       </c>
       <c r="E22" t="n">
         <v>0.03398225929140364</v>

</xml_diff>